<commit_message>
We fly high, no lie
URL je teď správně hypertext, eradikovány neznámé obory
</commit_message>
<xml_diff>
--- a/školy-zdroj.xlsx
+++ b/školy-zdroj.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/226e3371a49bebd4/Dokumenty/MFVS stuff/Erasmus-visual-streamlit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DB4F494-DF07-4BAF-AFF9-B552957E4534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{3DB4F494-DF07-4BAF-AFF9-B552957E4534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{789A5E4B-8246-46DC-BA16-EE18A01BE36A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
+    <sheet name="List1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2631" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2739" uniqueCount="585">
   <si>
     <t>interniNazevSmlouvy</t>
   </si>
@@ -2134,9 +2135,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BZ56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
+    <sheetView topLeftCell="AV1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AZ56" sqref="AZ3:AZ56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13154,4 +13155,458 @@
     <oddFooter>&amp;C&amp;P / &amp;N</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E46B0622-EB2B-42B1-8BE0-CA78E40C2073}">
+  <dimension ref="A1:B54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>374</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B54">
+    <sortCondition ref="A1:A54"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>